<commit_message>
--parametrized test case --added config.properties --written webdriver methods in BaseTestCase class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\titir_workspace\pwc_selenium_test\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCEFD55-EFF5-4000-9A47-8FD595EC0254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8511E97-9355-4E1F-9DD3-8E1506E10C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2550" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>FirstName</t>
   </si>
@@ -72,19 +72,25 @@
     <t>Sports</t>
   </si>
   <si>
-    <t>Kolkata</t>
-  </si>
-  <si>
-    <t>Garden Reach, Kolkata</t>
-  </si>
-  <si>
-    <t>West Bengal</t>
-  </si>
-  <si>
     <t>1234567890</t>
   </si>
   <si>
-    <t>12-12-1993</t>
+    <t>Subjects</t>
+  </si>
+  <si>
+    <t>Anything</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>Agra</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>03 Aug 1993</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +433,7 @@
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,19 +453,22 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -467,28 +476,31 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
       <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>